<commit_message>
req-v1 and specs v2 updated
</commit_message>
<xml_diff>
--- a/documentation/Specs_w_Estimates/Specs_v2.xlsx
+++ b/documentation/Specs_w_Estimates/Specs_v2.xlsx
@@ -24,14 +24,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="35">
   <si>
     <t>Specification</t>
   </si>
   <si>
-    <t>Calculate x and y distance using the start coordinates and exchange coordinates.</t>
-  </si>
-  <si>
     <t>Display “Home Address” at the (0,0) location on grid</t>
   </si>
   <si>
@@ -41,12 +38,6 @@
     <t>Total</t>
   </si>
   <si>
-    <t>IDs must be unique</t>
-  </si>
-  <si>
-    <t>Total the distance and output exchange ID with shortest distance</t>
-  </si>
-  <si>
     <t>If both distances are the same, output first ID</t>
   </si>
   <si>
@@ -68,9 +59,6 @@
     <t>(Setup)</t>
   </si>
   <si>
-    <t>Let User input 2 exchange locations by coordinate (w/ ID's in form ex:p:q)</t>
-  </si>
-  <si>
     <t>M4</t>
   </si>
   <si>
@@ -111,6 +99,36 @@
   </si>
   <si>
     <t>Use capacity of exchange when determining which to choose if equidistant</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>TODO</t>
+  </si>
+  <si>
+    <t>maybe</t>
+  </si>
+  <si>
+    <t>Exchange IDs must be unique</t>
+  </si>
+  <si>
+    <t>Let User input 2 exchanges</t>
+  </si>
+  <si>
+    <t>Let User input exchange format as an ID, x location, and y location</t>
+  </si>
+  <si>
+    <t>Calculate exchange distance as x + y location</t>
+  </si>
+  <si>
+    <t>Determine which exchange has smallest distance and output its ID</t>
+  </si>
+  <si>
+    <t>Validate exchange ID format "ex:[0-9]:[0-9]"</t>
   </si>
 </sst>
 </file>
@@ -165,7 +183,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -190,6 +208,30 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -224,7 +266,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
@@ -243,7 +285,14 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -529,10 +578,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -545,15 +594,18 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D1" t="s">
-        <v>12</v>
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C2" s="8">
         <v>0.5</v>
@@ -572,168 +624,223 @@
       <c r="D4" s="8"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="5" t="s">
+      <c r="A5" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="D5" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="D5" s="8">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A6" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="D6" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="D7" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="H7" s="4"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="D6" s="8">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="D7" s="8">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A8" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="D8" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="H8" s="4"/>
+      <c r="B8" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="D8" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A9" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="6" t="s">
+      <c r="A9" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="11"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="D10" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="11"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="D12" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="H12" s="4"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="D9" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="H9" s="4"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="D10" s="8">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A11" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="D11" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="H11" s="4"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A13" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D13" s="9"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A14" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C14" t="s">
+      <c r="B13" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D14" t="s">
-        <v>23</v>
-      </c>
+      <c r="C13" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="D13" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="H13" s="4"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="C15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" s="9"/>
+      <c r="E16" s="11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E18" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B17" s="4" t="s">
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B19" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" s="3">
+        <f>SUM(C2:C17)</f>
         <v>4</v>
       </c>
-      <c r="C17" s="3">
-        <f>SUM(C2:C15)</f>
-        <v>4</v>
-      </c>
-      <c r="D17" s="3">
-        <f>SUM(D5:D15)</f>
-        <v>3.5</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="C18" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B20" s="7"/>
+      <c r="D19" s="3">
+        <f>SUM(D10:D17)</f>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B22" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
specs: customer displayed in grid
</commit_message>
<xml_diff>
--- a/documentation/Specs_w_Estimates/Specs_v2.xlsx
+++ b/documentation/Specs_w_Estimates/Specs_v2.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="47">
   <si>
     <t>Display “Home Address” at the (0,0) location on grid</t>
   </si>
@@ -128,6 +128,9 @@
     <t>M9</t>
   </si>
   <si>
+    <t>M10</t>
+  </si>
+  <si>
     <t>VERSION3 VERSION3 VERSION3 VERSION3 VERSION3 VERSION3 VERSION3 VERSION3 VERSION3 VERSION3 VERSION3 VERSION3 VERSION3 VERSION3 VERSION3 VERSION3 VERSION3</t>
   </si>
   <si>
@@ -149,16 +152,19 @@
     <t>COULD HAVE</t>
   </si>
   <si>
-    <t xml:space="preserve">exchange ID and the distance from customer </t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
     <t>GRAND TOTAL</t>
   </si>
   <si>
-    <t xml:space="preserve">Whan calculate button clicked: Display grid where each grid cell that contains an exchange will display </t>
+    <t>Whan calculate button clicked: Display grid where each grid cell that contains an</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> exchange will display exchange ID and the distance from customer </t>
+  </si>
+  <si>
+    <t>Display customer in top left cell of grid</t>
   </si>
 </sst>
 </file>
@@ -506,7 +512,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
@@ -520,14 +526,12 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="13" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -539,9 +543,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="13" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -569,15 +570,8 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="15" borderId="9" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="15" borderId="13" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -587,6 +581,19 @@
     <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Calculation" xfId="3" builtinId="22"/>
@@ -619,7 +626,7 @@
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>116414</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>148169</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -764,7 +771,7 @@
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>148166</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1116,10 +1123,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N38"/>
+  <dimension ref="A1:N39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1152,16 +1159,16 @@
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
-      <c r="C2" s="49" t="s">
-        <v>39</v>
+      <c r="C2" s="43" t="s">
+        <v>40</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
-      <c r="I2" s="49" t="s">
-        <v>40</v>
+      <c r="I2" s="43" t="s">
+        <v>41</v>
       </c>
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
@@ -1187,62 +1194,62 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" s="3"/>
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="28" t="s">
+      <c r="C4" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="28" t="s">
+      <c r="D4" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="E4" s="28" t="s">
+      <c r="E4" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="F4" s="29"/>
+      <c r="F4" s="26"/>
       <c r="G4" s="3"/>
-      <c r="H4" s="27" t="s">
+      <c r="H4" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="I4" s="28" t="s">
+      <c r="I4" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="J4" s="28" t="s">
-        <v>38</v>
-      </c>
-      <c r="K4" s="28" t="s">
+      <c r="J4" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="K4" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="L4" s="29"/>
+      <c r="L4" s="26"/>
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" s="3"/>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="12"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="11"/>
       <c r="G5" s="3"/>
-      <c r="H5" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11"/>
-      <c r="K5" s="11"/>
-      <c r="L5" s="12"/>
+      <c r="H5" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="11"/>
       <c r="M5" s="3"/>
       <c r="N5" s="3"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" s="3"/>
-      <c r="B6" s="25" t="s">
+      <c r="B6" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="C6" s="15" t="s">
         <v>21</v>
       </c>
       <c r="D6" s="2">
@@ -1253,19 +1260,19 @@
       </c>
       <c r="F6" s="6"/>
       <c r="G6" s="3"/>
-      <c r="H6" s="30" t="s">
+      <c r="H6" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="I6" s="31" t="s">
+      <c r="I6" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="J6" s="32">
+      <c r="J6" s="29">
         <v>0.5</v>
       </c>
-      <c r="K6" s="32">
+      <c r="K6" s="29">
         <v>0.5</v>
       </c>
-      <c r="L6" s="33" t="s">
+      <c r="L6" s="30" t="s">
         <v>16</v>
       </c>
       <c r="M6" s="3"/>
@@ -1273,10 +1280,10 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" s="3"/>
-      <c r="B7" s="26" t="s">
+      <c r="B7" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="18" t="s">
+      <c r="C7" s="16" t="s">
         <v>2</v>
       </c>
       <c r="D7" s="1">
@@ -1287,19 +1294,19 @@
       </c>
       <c r="F7" s="7"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="34" t="s">
+      <c r="H7" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="I7" s="35" t="s">
+      <c r="I7" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="J7" s="36">
+      <c r="J7" s="33">
         <v>0.5</v>
       </c>
-      <c r="K7" s="36">
+      <c r="K7" s="33">
         <v>0.5</v>
       </c>
-      <c r="L7" s="33" t="s">
+      <c r="L7" s="30" t="s">
         <v>16</v>
       </c>
       <c r="M7" s="3"/>
@@ -1307,10 +1314,10 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" s="3"/>
-      <c r="B8" s="25" t="s">
+      <c r="B8" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="C8" s="15" t="s">
         <v>20</v>
       </c>
       <c r="D8" s="2">
@@ -1321,19 +1328,19 @@
       </c>
       <c r="F8" s="6"/>
       <c r="G8" s="3"/>
-      <c r="H8" s="30" t="s">
+      <c r="H8" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="I8" s="40" t="s">
+      <c r="I8" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="J8" s="32">
+      <c r="J8" s="29">
         <v>0.5</v>
       </c>
-      <c r="K8" s="32">
+      <c r="K8" s="29">
         <v>0.5</v>
       </c>
-      <c r="L8" s="33" t="s">
+      <c r="L8" s="30" t="s">
         <v>16</v>
       </c>
       <c r="M8" s="3"/>
@@ -1341,10 +1348,10 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" s="3"/>
-      <c r="B9" s="26" t="s">
+      <c r="B9" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="19" t="s">
+      <c r="C9" s="17" t="s">
         <v>17</v>
       </c>
       <c r="D9" s="1">
@@ -1355,22 +1362,22 @@
       </c>
       <c r="F9" s="7"/>
       <c r="G9" s="3"/>
-      <c r="H9" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="I9" s="11"/>
-      <c r="J9" s="11"/>
-      <c r="K9" s="11"/>
-      <c r="L9" s="12"/>
+      <c r="H9" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="11"/>
       <c r="M9" s="3"/>
       <c r="N9" s="3"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" s="3"/>
-      <c r="B10" s="25" t="s">
+      <c r="B10" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="17" t="s">
+      <c r="C10" s="15" t="s">
         <v>22</v>
       </c>
       <c r="D10" s="2">
@@ -1381,19 +1388,19 @@
       </c>
       <c r="F10" s="6"/>
       <c r="G10" s="3"/>
-      <c r="H10" s="37" t="s">
+      <c r="H10" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="I10" s="38" t="s">
+      <c r="I10" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="J10" s="47" t="s">
+      <c r="J10" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="K10" s="47" t="s">
+      <c r="K10" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="L10" s="39" t="s">
+      <c r="L10" s="36" t="s">
         <v>16</v>
       </c>
       <c r="M10" s="3"/>
@@ -1401,10 +1408,10 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" s="3"/>
-      <c r="B11" s="26" t="s">
+      <c r="B11" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="19" t="s">
+      <c r="C11" s="17" t="s">
         <v>11</v>
       </c>
       <c r="D11" s="1">
@@ -1417,13 +1424,13 @@
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
       <c r="I11" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="J11" s="43">
+        <v>36</v>
+      </c>
+      <c r="J11" s="39">
         <f>SUM(J6:J9)</f>
         <v>1.5</v>
       </c>
-      <c r="K11" s="44">
+      <c r="K11" s="40">
         <f>SUM(K6:K10)</f>
         <v>1.5</v>
       </c>
@@ -1433,10 +1440,10 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" s="3"/>
-      <c r="B12" s="25" t="s">
+      <c r="B12" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="20" t="s">
+      <c r="C12" s="18" t="s">
         <v>19</v>
       </c>
       <c r="D12" s="2">
@@ -1457,10 +1464,10 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" s="3"/>
-      <c r="B13" s="26" t="s">
+      <c r="B13" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="21" t="s">
+      <c r="C13" s="19" t="s">
         <v>18</v>
       </c>
       <c r="D13" s="1">
@@ -1481,13 +1488,13 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" s="3"/>
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="12"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="11"/>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
@@ -1499,16 +1506,16 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" s="3"/>
-      <c r="B15" s="24" t="s">
+      <c r="B15" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="41" t="s">
+      <c r="C15" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="D15" s="41">
+      <c r="D15" s="38">
         <v>0.25</v>
       </c>
-      <c r="E15" s="41">
+      <c r="E15" s="38">
         <v>0.5</v>
       </c>
       <c r="F15" s="8" t="s">
@@ -1525,13 +1532,13 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" s="3"/>
-      <c r="B16" s="16"/>
+      <c r="B16" s="21"/>
       <c r="C16" s="9" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="D16" s="9"/>
       <c r="E16" s="9"/>
-      <c r="F16" s="10"/>
+      <c r="F16" s="8"/>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
@@ -1544,12 +1551,16 @@
     <row r="17" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A17" s="3"/>
       <c r="B17" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="12"/>
+        <v>27</v>
+      </c>
+      <c r="C17" s="38" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17" s="38"/>
+      <c r="E17" s="38"/>
+      <c r="F17" s="8" t="s">
+        <v>16</v>
+      </c>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
@@ -1561,21 +1572,13 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A18" s="3"/>
-      <c r="B18" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D18" s="45" t="s">
-        <v>42</v>
-      </c>
-      <c r="E18" s="45" t="s">
-        <v>42</v>
-      </c>
-      <c r="F18" s="8" t="s">
-        <v>16</v>
-      </c>
+      <c r="B18" s="44" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="45"/>
+      <c r="D18" s="45"/>
+      <c r="E18" s="45"/>
+      <c r="F18" s="46"/>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
@@ -1587,16 +1590,24 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A19" s="3"/>
-      <c r="B19" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="12"/>
+      <c r="B19" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19" s="49" t="s">
+        <v>42</v>
+      </c>
+      <c r="E19" s="49" t="s">
+        <v>42</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>16</v>
+      </c>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
-      <c r="I19" s="4"/>
+      <c r="I19" s="3"/>
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
       <c r="L19" s="3"/>
@@ -1605,24 +1616,16 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A20" s="3"/>
-      <c r="B20" s="42" t="s">
-        <v>33</v>
-      </c>
-      <c r="C20" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="D20" s="46" t="s">
-        <v>42</v>
-      </c>
-      <c r="E20" s="46" t="s">
-        <v>42</v>
-      </c>
-      <c r="F20" s="23" t="s">
-        <v>16</v>
-      </c>
+      <c r="B20" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="11"/>
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
+      <c r="I20" s="4"/>
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
       <c r="L20" s="3"/>
@@ -1631,19 +1634,21 @@
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A21" s="3"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="D21" s="43">
-        <f>SUM(D6:D20)</f>
-        <v>3.5</v>
-      </c>
-      <c r="E21" s="44">
-        <f>SUM(E6:E20)</f>
-        <v>5</v>
-      </c>
-      <c r="F21" s="3"/>
+      <c r="B21" s="50" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" s="47" t="s">
+        <v>13</v>
+      </c>
+      <c r="D21" s="48" t="s">
+        <v>42</v>
+      </c>
+      <c r="E21" s="48" t="s">
+        <v>42</v>
+      </c>
+      <c r="F21" s="20" t="s">
+        <v>16</v>
+      </c>
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
@@ -1656,9 +1661,17 @@
     <row r="22" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
+      <c r="C22" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D22" s="39">
+        <f>SUM(D6:D21)</f>
+        <v>3.5</v>
+      </c>
+      <c r="E22" s="40">
+        <f>SUM(E6:E21)</f>
+        <v>5</v>
+      </c>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
@@ -1669,7 +1682,7 @@
       <c r="M22" s="3"/>
       <c r="N22" s="3"/>
     </row>
-    <row r="23" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -1688,14 +1701,9 @@
     <row r="24" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="E24" s="48">
-        <f>SUM(D21+E21)</f>
-        <v>8.5</v>
-      </c>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
@@ -1706,12 +1714,17 @@
       <c r="M24" s="3"/>
       <c r="N24" s="3"/>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E25" s="42">
+        <f>SUM(D22+E22)</f>
+        <v>8.5</v>
+      </c>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
@@ -1930,6 +1943,22 @@
       <c r="M38" s="3"/>
       <c r="N38" s="3"/>
     </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A39" s="3"/>
+      <c r="B39" s="3"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="3"/>
+      <c r="H39" s="3"/>
+      <c r="I39" s="3"/>
+      <c r="J39" s="3"/>
+      <c r="K39" s="3"/>
+      <c r="L39" s="3"/>
+      <c r="M39" s="3"/>
+      <c r="N39" s="3"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
specs and pres tuesday
</commit_message>
<xml_diff>
--- a/documentation/Specs_w_Estimates/Specs_v2.xlsx
+++ b/documentation/Specs_w_Estimates/Specs_v2.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="55">
   <si>
     <t>Display “Home Address” at the (0,0) location on grid</t>
   </si>
@@ -119,9 +119,6 @@
     <t>TEST TIME</t>
   </si>
   <si>
-    <t>Let user input up to 99 exchanges</t>
-  </si>
-  <si>
     <t>VERSION4 VERSION4 VERSION4 VERSION4 VERSION4 VERSION4 VERSION4 VERSION4 VERSION4 VERSION4 VERSION4 VERSION4 VERSION4 VERSION4 VERSION4 VERSION4 VERSION4</t>
   </si>
   <si>
@@ -165,6 +162,33 @@
   </si>
   <si>
     <t>Display customer in top left cell of grid</t>
+  </si>
+  <si>
+    <t>Let user input up to 99 exchanges [add button]</t>
+  </si>
+  <si>
+    <t>C5</t>
+  </si>
+  <si>
+    <t>Reset button</t>
+  </si>
+  <si>
+    <t>Placeholder text</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>S2</t>
+  </si>
+  <si>
+    <t>Format exchange entry to new design</t>
+  </si>
+  <si>
+    <t>populate dropdown with added exchanges</t>
+  </si>
+  <si>
+    <t>VERSION3 VERSION3 VERSION3 VERSION3 VERSION3 VERSION3 VERSION3 VERSION3 VERSION3 VERSION3 VERSION3 VERSION</t>
   </si>
 </sst>
 </file>
@@ -246,7 +270,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -334,6 +358,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="15">
     <border>
@@ -512,7 +548,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
@@ -590,7 +626,13 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Calculation" xfId="3" builtinId="22"/>
@@ -609,252 +651,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>46562</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>3</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>116414</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>148169</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="Oval 3"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="12090395" y="2698753"/>
-          <a:ext cx="4779436" cy="2688166"/>
-        </a:xfrm>
-        <a:prstGeom prst="ellipse">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="00B050"/>
-        </a:solidFill>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-GB" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>15476</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>168668</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>93199</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
-          <a:duotone>
-            <a:schemeClr val="accent4">
-              <a:shade val="45000"/>
-              <a:satMod val="135000"/>
-            </a:schemeClr>
-            <a:prstClr val="white"/>
-          </a:duotone>
-          <a:extLst>
-            <a:ext uri="{BEBA8EAE-BF5A-486C-A8C5-ECC9F3942E4B}">
-              <a14:imgProps xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-                <a14:imgLayer r:embed="rId2">
-                  <a14:imgEffect>
-                    <a14:brightnessContrast bright="86000"/>
-                  </a14:imgEffect>
-                </a14:imgLayer>
-              </a14:imgProps>
-            </a:ext>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="12059309" y="2667000"/>
-          <a:ext cx="4862776" cy="2813116"/>
-        </a:xfrm>
-        <a:prstGeom prst="ellipse">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent2">
-            <a:lumMod val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:ln w="190500" cap="rnd">
-          <a:solidFill>
-            <a:srgbClr val="C8C6BD"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst>
-          <a:outerShdw blurRad="127000" algn="bl" rotWithShape="0">
-            <a:srgbClr val="000000"/>
-          </a:outerShdw>
-        </a:effectLst>
-        <a:scene3d>
-          <a:camera prst="perspectiveFront" fov="5400000"/>
-          <a:lightRig rig="threePt" dir="t">
-            <a:rot lat="0" lon="0" rev="19200000"/>
-          </a:lightRig>
-        </a:scene3d>
-        <a:sp3d extrusionH="25400">
-          <a:bevelT w="304800" h="152400" prst="hardEdge"/>
-          <a:extrusionClr>
-            <a:srgbClr val="000000"/>
-          </a:extrusionClr>
-        </a:sp3d>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>836084</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>148166</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="TextBox 1"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="12879917" y="2518833"/>
-          <a:ext cx="4021666" cy="2603500"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="9525" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst>
-          <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
-            <a:prstClr val="black">
-              <a:alpha val="40000"/>
-            </a:prstClr>
-          </a:outerShdw>
-        </a:effectLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-GB" sz="4400" u="sng">
-              <a:latin typeface="Agency FB" panose="020B0503020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>Team </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-GB" sz="8800" b="0" i="0" u="sng">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="Agency FB" panose="020B0503020202020204" pitchFamily="34" charset="0"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>∞</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-GB" sz="5400" b="0" i="0" u="none">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="Agency FB" panose="020B0503020202020204" pitchFamily="34" charset="0"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>Specifications</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-GB" sz="4800" u="none">
-            <a:latin typeface="Agency FB" panose="020B0503020202020204" pitchFamily="34" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1123,7 +919,7 @@
   <dimension ref="A1:N39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1157,7 +953,7 @@
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="43" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
@@ -1165,7 +961,7 @@
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
       <c r="I2" s="43" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
@@ -1212,7 +1008,7 @@
         <v>24</v>
       </c>
       <c r="J4" s="25" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K4" s="25" t="s">
         <v>30</v>
@@ -1232,7 +1028,7 @@
       <c r="F5" s="11"/>
       <c r="G5" s="3"/>
       <c r="H5" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I5" s="10"/>
       <c r="J5" s="10"/>
@@ -1360,7 +1156,7 @@
       <c r="F9" s="7"/>
       <c r="G9" s="3"/>
       <c r="H9" s="12" t="s">
-        <v>38</v>
+        <v>54</v>
       </c>
       <c r="I9" s="10"/>
       <c r="J9" s="10"/>
@@ -1385,19 +1181,15 @@
       </c>
       <c r="F10" s="6"/>
       <c r="G10" s="3"/>
-      <c r="H10" s="34" t="s">
+      <c r="H10" s="50" t="s">
         <v>14</v>
       </c>
-      <c r="I10" s="35" t="s">
-        <v>15</v>
-      </c>
-      <c r="J10" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="K10" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="L10" s="36" t="s">
+      <c r="I10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="51" t="s">
         <v>16</v>
       </c>
       <c r="M10" s="3"/>
@@ -1419,19 +1211,17 @@
       </c>
       <c r="F11" s="7"/>
       <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="J11" s="39">
-        <f>SUM(J6:J9)</f>
-        <v>1.5</v>
-      </c>
-      <c r="K11" s="40">
-        <f>SUM(K6:K10)</f>
-        <v>1.5</v>
-      </c>
-      <c r="L11" s="3"/>
+      <c r="H11" s="47" t="s">
+        <v>47</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="8" t="s">
+        <v>16</v>
+      </c>
       <c r="M11" s="3"/>
       <c r="N11" s="3"/>
     </row>
@@ -1475,8 +1265,12 @@
       </c>
       <c r="F13" s="7"/>
       <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="4"/>
+      <c r="H13" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="I13" s="49" t="s">
+        <v>52</v>
+      </c>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
@@ -1493,8 +1287,12 @@
       <c r="E14" s="10"/>
       <c r="F14" s="11"/>
       <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
+      <c r="H14" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>53</v>
+      </c>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
@@ -1507,17 +1305,15 @@
         <v>23</v>
       </c>
       <c r="C15" s="38" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D15" s="38">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="E15" s="38">
         <v>0.5</v>
       </c>
-      <c r="F15" s="8" t="s">
-        <v>16</v>
-      </c>
+      <c r="F15" s="6"/>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
@@ -1531,17 +1327,19 @@
       <c r="A16" s="3"/>
       <c r="B16" s="21"/>
       <c r="C16" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D16" s="9"/>
       <c r="E16" s="9"/>
-      <c r="F16" s="8"/>
+      <c r="F16" s="6"/>
       <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
-      <c r="L16" s="3"/>
+      <c r="H16" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="11"/>
       <c r="M16" s="3"/>
       <c r="N16" s="3"/>
     </row>
@@ -1551,26 +1349,38 @@
         <v>27</v>
       </c>
       <c r="C17" s="38" t="s">
-        <v>46</v>
-      </c>
-      <c r="D17" s="38"/>
-      <c r="E17" s="38"/>
-      <c r="F17" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D17" s="38">
+        <v>0.25</v>
+      </c>
+      <c r="E17" s="38">
+        <v>0.5</v>
+      </c>
+      <c r="F17" s="7"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="I17" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="J17" s="41" t="s">
+        <v>41</v>
+      </c>
+      <c r="K17" s="41" t="s">
+        <v>41</v>
+      </c>
+      <c r="L17" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
-      <c r="L17" s="3"/>
       <c r="M17" s="3"/>
       <c r="N17" s="3"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A18" s="3"/>
       <c r="B18" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
@@ -1578,9 +1388,17 @@
       <c r="F18" s="11"/>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
+      <c r="I18" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="J18" s="39">
+        <f>SUM(J6:J16)</f>
+        <v>1.5</v>
+      </c>
+      <c r="K18" s="40">
+        <f>SUM(K6:K17)</f>
+        <v>1.5</v>
+      </c>
       <c r="L18" s="3"/>
       <c r="M18" s="3"/>
       <c r="N18" s="3"/>
@@ -1588,16 +1406,16 @@
     <row r="19" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A19" s="3"/>
       <c r="B19" s="21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="D19" s="46" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E19" s="46" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F19" s="8" t="s">
         <v>16</v>
@@ -1614,7 +1432,7 @@
     <row r="20" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A20" s="3"/>
       <c r="B20" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C20" s="10"/>
       <c r="D20" s="10"/>
@@ -1631,17 +1449,17 @@
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A21" s="3"/>
-      <c r="B21" s="47" t="s">
-        <v>34</v>
+      <c r="B21" s="48" t="s">
+        <v>33</v>
       </c>
       <c r="C21" s="44" t="s">
         <v>13</v>
       </c>
       <c r="D21" s="45" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E21" s="45" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F21" s="20" t="s">
         <v>16</v>
@@ -1659,15 +1477,15 @@
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D22" s="39">
         <f>SUM(D6:D21)</f>
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="E22" s="40">
         <f>SUM(E6:E21)</f>
-        <v>5</v>
+        <v>5.5</v>
       </c>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
@@ -1716,11 +1534,11 @@
       <c r="B25" s="3"/>
       <c r="C25" s="5"/>
       <c r="D25" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E25" s="42">
         <f>SUM(D22+E22)</f>
-        <v>8.5</v>
+        <v>9.5</v>
       </c>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
@@ -1959,6 +1777,5 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>